<commit_message>
Your message describing the changes
</commit_message>
<xml_diff>
--- a/admin/ajax/faculty_format (3).xlsx
+++ b/admin/ajax/faculty_format (3).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11580"/>
+    <workbookView windowWidth="21000" windowHeight="11130"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -87,13 +87,13 @@
     <t>Consultation Time</t>
   </si>
   <si>
-    <t>Hanz Jansen</t>
+    <t>Hanz Jansen123</t>
   </si>
   <si>
     <t>IT DEPARTMENT</t>
   </si>
   <si>
-    <t>dwadwadwadwadwawdawadwadw</t>
+    <t>batmat</t>
   </si>
 </sst>
 </file>
@@ -1071,13 +1071,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="15.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="33.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="10.5714285714286"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1097,8 +1102,19 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>123412313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>